<commit_message>
completed Enviorment Variable for two different ESP32 types
</commit_message>
<xml_diff>
--- a/PinAssingments.xlsx
+++ b/PinAssingments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Capplegate\GitHub\Freezy Estops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06274BC5-13C2-46F1-AC19-02F11F1835DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9094CB22-A2EE-4CE7-8F23-6DA7B67EE309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A9BD991A-3096-485E-A4B4-87AF2E5C8E9C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="182">
   <si>
     <t>Field Stop</t>
   </si>
@@ -579,6 +579,9 @@
   </si>
   <si>
     <t>Freezy Assinment</t>
+  </si>
+  <si>
+    <t>Start Match</t>
   </si>
 </sst>
 </file>
@@ -675,7 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -690,22 +693,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -721,7 +724,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="220">
+  <dxfs count="84">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -739,6 +756,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -788,6 +812,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -802,7 +840,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -816,7 +868,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -830,7 +896,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -858,6 +938,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9"/>
         </patternFill>
       </fill>
@@ -872,7 +959,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -886,1073 +987,15 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2063,7 +1106,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2099,20 +1142,6 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2139,24 +1168,17 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2192,6 +1214,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2225,6 +1250,23 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2248,14 +1290,9 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2283,11 +1320,50 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
         <top/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2316,12 +1392,17 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
         <top/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2349,25 +1430,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
         <top/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -2397,6 +1466,19 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2434,6 +1516,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2469,6 +1554,23 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2493,14 +1595,14 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
         <right style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </right>
         <top/>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2529,9 +1631,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
+        <right/>
         <top/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -2564,14 +1664,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
+        <right/>
         <top/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2599,14 +1700,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
+        <right/>
         <top/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2633,25 +1735,34 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top/>
-        <bottom/>
+        </top>
       </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2661,56 +1772,18 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2726,43 +1799,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F634E3CE-C995-4DA1-9079-A7A2401AA8F6}" name="Table5" displayName="Table5" ref="I2:L43" headerRowCount="0" totalsRowShown="0" headerRowDxfId="187" dataDxfId="186" headerRowBorderDxfId="184" tableBorderDxfId="185">
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A251C808-FC9C-4EF4-9DD8-E2A5656F3791}" name="Column1" headerRowDxfId="183" dataDxfId="182"/>
-    <tableColumn id="3" xr3:uid="{A5DC1262-CD6F-475D-96AC-1C51B0331EF0}" name="Column3" headerRowDxfId="181" dataDxfId="180"/>
-    <tableColumn id="4" xr3:uid="{69DAEA7C-5786-4619-82E7-7EE5426B794A}" name="Column4" headerRowDxfId="179" dataDxfId="178"/>
-    <tableColumn id="5" xr3:uid="{98293955-D638-4A82-8BE6-AB516B4E9D4B}" name="Column5" headerRowDxfId="177" dataDxfId="176"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F634E3CE-C995-4DA1-9079-A7A2401AA8F6}" name="Table5" displayName="Table5" ref="I2:M43" headerRowCount="0" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80">
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A251C808-FC9C-4EF4-9DD8-E2A5656F3791}" name="Column1" headerRowDxfId="79" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{A5DC1262-CD6F-475D-96AC-1C51B0331EF0}" name="Column3" headerRowDxfId="77" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{69DAEA7C-5786-4619-82E7-7EE5426B794A}" name="Column4" headerRowDxfId="75" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{941267CE-BE97-4490-AE30-41FCDDB954D7}" name="Column2" headerRowDxfId="41" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{98293955-D638-4A82-8BE6-AB516B4E9D4B}" name="Column5" headerRowDxfId="74" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5B838371-7118-4D1E-83EA-FB9A8A4ADD02}" name="Table7" displayName="Table7" ref="O2:T43" headerRowCount="0" totalsRowShown="0" headerRowDxfId="210" dataDxfId="211" headerRowBorderDxfId="218" tableBorderDxfId="219">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5B838371-7118-4D1E-83EA-FB9A8A4ADD02}" name="Table7" displayName="Table7" ref="P2:U43" headerRowCount="0" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{213E74EC-EABF-4790-B9F3-D1FD8946CB37}" name="Column1" headerRowDxfId="204" dataDxfId="217"/>
-    <tableColumn id="2" xr3:uid="{A8DA0FDA-73EE-4565-82BE-627AF672B314}" name="Column2" headerRowDxfId="205" dataDxfId="216"/>
-    <tableColumn id="3" xr3:uid="{4B7356FF-2B95-4F95-9D69-8D3E014BBAFA}" name="Column3" headerRowDxfId="206" dataDxfId="215"/>
-    <tableColumn id="4" xr3:uid="{AAEB758F-7A52-4D9D-B98E-A2B1B5A79459}" name="Column4" headerRowDxfId="207" dataDxfId="214"/>
-    <tableColumn id="5" xr3:uid="{5C8EFBE9-8AA6-4C38-A832-D6F365795A0F}" name="Column5" headerRowDxfId="208" dataDxfId="213"/>
-    <tableColumn id="6" xr3:uid="{F9F1319E-9185-464B-AE0E-7295E577FFE4}" name="Column6" headerRowDxfId="209" dataDxfId="212"/>
+    <tableColumn id="1" xr3:uid="{213E74EC-EABF-4790-B9F3-D1FD8946CB37}" name="Column1" headerRowDxfId="69" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{A8DA0FDA-73EE-4565-82BE-627AF672B314}" name="Column2" headerRowDxfId="67" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{4B7356FF-2B95-4F95-9D69-8D3E014BBAFA}" name="Column3" headerRowDxfId="65" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{AAEB758F-7A52-4D9D-B98E-A2B1B5A79459}" name="Column4" headerRowDxfId="63" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{5C8EFBE9-8AA6-4C38-A832-D6F365795A0F}" name="Column5" headerRowDxfId="61" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{F9F1319E-9185-464B-AE0E-7295E577FFE4}" name="Column6" headerRowDxfId="59" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{954ECF6F-E537-4021-B32A-D6174B508832}" name="Table59" displayName="Table59" ref="B2:G53" headerRowCount="0" totalsRowShown="0" headerRowDxfId="203" dataDxfId="202" headerRowBorderDxfId="200" tableBorderDxfId="201">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{954ECF6F-E537-4021-B32A-D6174B508832}" name="Table59" displayName="Table59" ref="B2:G53" headerRowCount="0" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:G53">
     <sortCondition ref="D4:D53"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00C203F6-5A2E-4106-B827-0D3AA3A9EAB7}" name="Column1" headerRowDxfId="199" dataDxfId="192"/>
-    <tableColumn id="6" xr3:uid="{0C1AFA47-59C0-4DC0-AA5D-62D755CBCA91}" name="Column2" headerRowDxfId="195" dataDxfId="191"/>
-    <tableColumn id="3" xr3:uid="{1ED9DD68-F4DF-4A5B-B9BE-348A2806A2F8}" name="Column3" headerRowDxfId="198" dataDxfId="190"/>
-    <tableColumn id="4" xr3:uid="{BF6BB523-56D0-4B45-9746-C89C1BC5AFCD}" name="Column4" headerRowDxfId="197" dataDxfId="189"/>
-    <tableColumn id="7" xr3:uid="{756A3636-1E62-4709-AF31-59895574C214}" name="Column6" headerRowDxfId="194" dataDxfId="188"/>
-    <tableColumn id="5" xr3:uid="{914009BC-2C9B-4814-B37A-9F4619F4AF69}" name="Column5" headerRowDxfId="196" dataDxfId="193"/>
+    <tableColumn id="1" xr3:uid="{00C203F6-5A2E-4106-B827-0D3AA3A9EAB7}" name="Column1" headerRowDxfId="53" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{0C1AFA47-59C0-4DC0-AA5D-62D755CBCA91}" name="Column2" headerRowDxfId="51" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{1ED9DD68-F4DF-4A5B-B9BE-348A2806A2F8}" name="Column3" headerRowDxfId="49" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{BF6BB523-56D0-4B45-9746-C89C1BC5AFCD}" name="Column4" headerRowDxfId="47" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{756A3636-1E62-4709-AF31-59895574C214}" name="Column6" headerRowDxfId="45" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{914009BC-2C9B-4814-B37A-9F4619F4AF69}" name="Column5" headerRowDxfId="43" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3085,10 +2159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBBFC3FA-690A-4FCF-BD50-AFE48694E174}">
-  <dimension ref="B1:T53"/>
+  <dimension ref="B1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3104,8 +2178,8 @@
     <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="60" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="60" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -3116,12 +2190,12 @@
     <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E1"/>
       <c r="F1" s="15"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>140</v>
       </c>
@@ -3137,18 +2211,18 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="3"/>
+      <c r="M2" s="4"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U2" s="11"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
@@ -3174,28 +2248,30 @@
       <c r="K3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>104</v>
       </c>
@@ -3207,9 +2283,6 @@
       </c>
       <c r="E4" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="1"/>
@@ -3222,31 +2295,30 @@
       <c r="K4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="3">
+      <c r="P4" s="3">
         <v>25</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="R4" s="1">
+      <c r="S4" s="1">
         <v>0</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="T4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>141</v>
       </c>
@@ -3258,9 +2330,6 @@
       </c>
       <c r="E5" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="1"/>
@@ -3273,31 +2342,30 @@
       <c r="K5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="3">
+      <c r="P5" s="3">
         <v>35</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="R5" s="1">
+      <c r="S5" s="1">
         <v>1</v>
       </c>
-      <c r="S5" s="8" t="s">
+      <c r="T5" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="U5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
@@ -3309,9 +2377,6 @@
       </c>
       <c r="E6" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="1"/>
@@ -3324,31 +2389,30 @@
       <c r="K6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="3">
+      <c r="P6" s="3">
         <v>24</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="R6" s="1">
+      <c r="S6" s="1">
         <v>2</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="T6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="U6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>142</v>
       </c>
@@ -3360,9 +2424,6 @@
       </c>
       <c r="E7" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="1"/>
@@ -3375,31 +2436,30 @@
       <c r="K7" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="3">
+      <c r="P7" s="3">
         <v>34</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S7" s="1">
         <v>3</v>
       </c>
-      <c r="S7" s="8" t="s">
+      <c r="T7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="U7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>169</v>
       </c>
@@ -3412,9 +2472,7 @@
       <c r="E8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
@@ -3426,29 +2484,28 @@
       <c r="K8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3">
+      <c r="M8" s="3"/>
+      <c r="P8" s="3">
         <v>26</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="R8" s="1">
+      <c r="S8" s="1">
         <v>4</v>
       </c>
-      <c r="S8" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T8" s="3"/>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U8" s="3"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>170</v>
       </c>
@@ -3461,9 +2518,7 @@
       <c r="E9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
@@ -3475,31 +2530,30 @@
       <c r="K9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="3">
+      <c r="P9" s="3">
         <v>29</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="R9" s="1">
+      <c r="S9" s="1">
         <v>5</v>
       </c>
-      <c r="S9" s="7" t="s">
+      <c r="T9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="T9" s="3" t="s">
+      <c r="U9" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>171</v>
       </c>
@@ -3512,9 +2566,7 @@
       <c r="E10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
@@ -3526,31 +2578,30 @@
       <c r="K10" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="3">
+      <c r="P10" s="3">
         <v>20</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="R10" s="1">
+      <c r="S10" s="1">
         <v>6</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="T10" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="T10" s="3" t="s">
+      <c r="U10" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>172</v>
       </c>
@@ -3563,7 +2614,7 @@
       <c r="E11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
@@ -3575,31 +2626,30 @@
       <c r="K11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="3">
+      <c r="P11" s="3">
         <v>21</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="R11" s="1">
+      <c r="S11" s="1">
         <v>7</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="T11" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="T11" s="3" t="s">
+      <c r="U11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="13">
         <v>8</v>
@@ -3610,7 +2660,7 @@
       <c r="E12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
@@ -3622,31 +2672,30 @@
       <c r="K12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="3">
+      <c r="P12" s="3">
         <v>22</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="R12" s="1">
+      <c r="S12" s="1">
         <v>8</v>
       </c>
-      <c r="S12" s="8" t="s">
+      <c r="T12" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="T12" s="3" t="s">
+      <c r="U12" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>173</v>
       </c>
@@ -3671,31 +2720,30 @@
       <c r="K13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="3">
+      <c r="P13" s="3">
         <v>17</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="Q13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="R13" s="1">
+      <c r="S13" s="1">
         <v>9</v>
       </c>
-      <c r="S13" s="8" t="s">
+      <c r="T13" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="T13" s="3" t="s">
+      <c r="U13" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>174</v>
       </c>
@@ -3720,31 +2768,30 @@
       <c r="K14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="M14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M14" s="3"/>
       <c r="N14" s="3"/>
-      <c r="O14" s="3">
+      <c r="P14" s="3">
         <v>18</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R14" s="1">
+      <c r="S14" s="1">
         <v>10</v>
       </c>
-      <c r="S14" s="8" t="s">
+      <c r="T14" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="T14" s="3" t="s">
+      <c r="U14" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>175</v>
       </c>
@@ -3769,31 +2816,30 @@
       <c r="K15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="M15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M15" s="3"/>
       <c r="N15" s="3"/>
-      <c r="O15" s="3">
+      <c r="P15" s="3">
         <v>19</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="R15" s="1">
+      <c r="S15" s="1">
         <v>11</v>
       </c>
-      <c r="S15" s="8" t="s">
+      <c r="T15" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="T15" s="3" t="s">
+      <c r="U15" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>176</v>
       </c>
@@ -3818,31 +2864,30 @@
       <c r="K16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="3"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="3">
+      <c r="P16" s="3">
         <v>14</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="Q16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="R16" s="1">
+      <c r="S16" s="1">
         <v>12</v>
       </c>
-      <c r="S16" s="10" t="s">
+      <c r="T16" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="T16" s="3" t="s">
+      <c r="U16" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>177</v>
       </c>
@@ -3867,25 +2912,24 @@
       <c r="K17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="3">
+      <c r="P17" s="3">
         <v>16</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="R17" s="1">
+      <c r="S17" s="1">
         <v>13</v>
       </c>
-      <c r="S17" s="9"/>
-      <c r="T17" s="3"/>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T17" s="9"/>
+      <c r="U17" s="3"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>178</v>
       </c>
@@ -3910,27 +2954,26 @@
       <c r="K18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="3">
+      <c r="P18" s="3">
         <v>13</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="R18" s="1">
+      <c r="S18" s="1">
         <v>14</v>
       </c>
-      <c r="S18" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T18" s="3"/>
-    </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U18" s="3"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>101</v>
       </c>
@@ -3954,31 +2997,30 @@
       <c r="K19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="M19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M19" s="3"/>
       <c r="N19" s="3"/>
-      <c r="O19" s="3">
+      <c r="P19" s="3">
         <v>23</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="Q19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="R19" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R19" s="1">
+      <c r="S19" s="1">
         <v>15</v>
       </c>
-      <c r="S19" s="7" t="s">
+      <c r="T19" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="T19" s="3" t="s">
+      <c r="U19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>107</v>
       </c>
@@ -4002,27 +3044,26 @@
       <c r="K20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="3">
+      <c r="P20" s="3">
         <v>27</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="R20" s="1">
+      <c r="S20" s="1">
         <v>16</v>
       </c>
-      <c r="S20" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T20" s="3"/>
-    </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T20" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U20" s="3"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>109</v>
       </c>
@@ -4046,27 +3087,26 @@
       <c r="K21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="3">
+      <c r="P21" s="3">
         <v>28</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="Q21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="R21" s="1">
+      <c r="S21" s="1">
         <v>17</v>
       </c>
-      <c r="S21" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T21" s="3"/>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U21" s="3"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>113</v>
       </c>
@@ -4090,27 +3130,26 @@
       <c r="K22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="3">
+      <c r="P22" s="3">
         <v>30</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="R22" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="R22" s="1">
+      <c r="S22" s="1">
         <v>18</v>
       </c>
-      <c r="S22" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T22" s="3"/>
-    </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T22" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U22" s="3"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>115</v>
       </c>
@@ -4134,27 +3173,29 @@
       <c r="K23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L23" s="3"/>
+      <c r="L23" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="3">
+      <c r="P23" s="3">
         <v>31</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="R23" s="1">
+      <c r="S23" s="1">
         <v>19</v>
       </c>
-      <c r="S23" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T23" s="3"/>
-    </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U23" s="3"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>143</v>
       </c>
@@ -4172,19 +3213,19 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="3"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="6"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
-      <c r="R24" s="5">
+      <c r="R24" s="6"/>
+      <c r="S24" s="5">
         <v>20</v>
       </c>
-      <c r="S24" s="6"/>
       <c r="T24" s="6"/>
-    </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U24" s="6"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>117</v>
       </c>
@@ -4211,27 +3252,29 @@
       <c r="K25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L25" s="3"/>
+      <c r="L25" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-      <c r="O25" s="3">
+      <c r="P25" s="3">
         <v>33</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="R25" s="1">
+      <c r="S25" s="1">
         <v>21</v>
       </c>
-      <c r="S25" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T25" s="3"/>
-    </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U25" s="3"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="13">
         <v>22</v>
@@ -4250,27 +3293,29 @@
       <c r="K26" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L26" s="3"/>
+      <c r="L26" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="3">
+      <c r="P26" s="3">
         <v>36</v>
       </c>
-      <c r="P26" s="1" t="s">
+      <c r="Q26" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="Q26" s="1" t="s">
+      <c r="R26" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="R26" s="1">
+      <c r="S26" s="1">
         <v>22</v>
       </c>
-      <c r="S26" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T26" s="3"/>
-    </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T26" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U26" s="3"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="13">
         <v>23</v>
@@ -4289,27 +3334,29 @@
       <c r="K27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L27" s="3"/>
+      <c r="L27" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="3">
+      <c r="P27" s="3">
         <v>37</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="R27" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="R27" s="1">
+      <c r="S27" s="1">
         <v>23</v>
       </c>
-      <c r="S27" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T27" s="3"/>
-    </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T27" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U27" s="3"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="13">
         <v>24</v>
@@ -4328,17 +3375,19 @@
       <c r="K28" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L28" s="3"/>
+      <c r="L28" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
-      <c r="O28" s="6"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="5"/>
       <c r="T28" s="6"/>
-    </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U28" s="6"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="13">
         <v>25</v>
@@ -4357,27 +3406,29 @@
       <c r="K29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L29" s="3"/>
+      <c r="L29" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
-      <c r="O29" s="3">
+      <c r="P29" s="3">
         <v>10</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="Q29" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="R29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R29" s="1">
+      <c r="S29" s="1">
         <v>25</v>
       </c>
-      <c r="S29" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T29" s="3"/>
-    </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T29" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U29" s="3"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="13">
         <v>26</v>
@@ -4398,27 +3449,29 @@
       <c r="K30" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L30" s="3"/>
+      <c r="L30" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="3">
+      <c r="P30" s="3">
         <v>11</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="Q30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R30" s="1">
+      <c r="S30" s="1">
         <v>26</v>
       </c>
-      <c r="S30" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T30" s="3"/>
-    </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U30" s="3"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="13">
         <v>27</v>
@@ -4437,27 +3490,29 @@
       <c r="K31" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L31" s="3"/>
+      <c r="L31" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="3">
+      <c r="P31" s="3">
         <v>12</v>
       </c>
-      <c r="P31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="R31" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R31" s="1">
+      <c r="S31" s="1">
         <v>27</v>
       </c>
-      <c r="S31" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T31" s="3"/>
-    </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T31" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U31" s="3"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="13">
         <v>28</v>
@@ -4470,19 +3525,19 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="3"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="6"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="6"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
-      <c r="R32" s="5">
+      <c r="R32" s="6"/>
+      <c r="S32" s="5">
         <v>28</v>
       </c>
-      <c r="S32" s="6"/>
       <c r="T32" s="6"/>
-    </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U32" s="6"/>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="13">
         <v>29</v>
@@ -4495,19 +3550,19 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="3"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="6"/>
       <c r="N33" s="3"/>
-      <c r="O33" s="6"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
-      <c r="R33" s="5">
+      <c r="R33" s="6"/>
+      <c r="S33" s="5">
         <v>29</v>
       </c>
-      <c r="S33" s="6"/>
       <c r="T33" s="6"/>
-    </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U33" s="6"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="13">
         <v>30</v>
@@ -4520,19 +3575,19 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="3"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="6"/>
       <c r="N34" s="3"/>
-      <c r="O34" s="6"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
-      <c r="R34" s="5">
+      <c r="R34" s="6"/>
+      <c r="S34" s="5">
         <v>30</v>
       </c>
-      <c r="S34" s="6"/>
       <c r="T34" s="6"/>
-    </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U34" s="6"/>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="13">
         <v>31</v>
@@ -4545,19 +3600,19 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="3"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="6"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="6"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="6"/>
-      <c r="R35" s="5">
+      <c r="R35" s="6"/>
+      <c r="S35" s="5">
         <v>31</v>
       </c>
-      <c r="S35" s="6"/>
       <c r="T35" s="6"/>
-    </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U35" s="6"/>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="13">
         <v>32</v>
@@ -4570,27 +3625,27 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="3"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="6"/>
       <c r="N36" s="3"/>
-      <c r="O36" s="3">
+      <c r="P36" s="3">
         <v>8</v>
       </c>
-      <c r="P36" s="1" t="s">
+      <c r="Q36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q36" s="1" t="s">
+      <c r="R36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="R36" s="1">
+      <c r="S36" s="1">
         <v>32</v>
       </c>
-      <c r="S36" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T36" s="3"/>
-    </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T36" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U36" s="3"/>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>75</v>
       </c>
@@ -4602,6 +3657,9 @@
       </c>
       <c r="E37" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="G37" s="9"/>
       <c r="H37" s="1"/>
@@ -4614,27 +3672,26 @@
       <c r="K37" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
-      <c r="O37" s="3">
+      <c r="P37" s="3">
         <v>9</v>
       </c>
-      <c r="P37" s="1" t="s">
+      <c r="Q37" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q37" s="1" t="s">
+      <c r="R37" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="R37" s="1">
+      <c r="S37" s="1">
         <v>33</v>
       </c>
-      <c r="S37" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T37" s="3"/>
-    </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T37" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U37" s="3"/>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>69</v>
       </c>
@@ -4646,6 +3703,9 @@
       </c>
       <c r="E38" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="G38" s="9"/>
       <c r="H38" s="1"/>
@@ -4658,31 +3718,30 @@
       <c r="K38" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L38" s="3" t="s">
+      <c r="M38" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M38" s="3"/>
       <c r="N38" s="3"/>
-      <c r="O38" s="3">
+      <c r="P38" s="3">
         <v>6</v>
       </c>
-      <c r="P38" s="1" t="s">
+      <c r="Q38" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q38" s="1" t="s">
+      <c r="R38" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="R38" s="1">
+      <c r="S38" s="1">
         <v>34</v>
       </c>
-      <c r="S38" s="7" t="s">
+      <c r="T38" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="T38" s="3" t="s">
+      <c r="U38" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>71</v>
       </c>
@@ -4694,6 +3753,9 @@
       </c>
       <c r="E39" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="G39" s="9"/>
       <c r="H39" s="1"/>
@@ -4706,31 +3768,30 @@
       <c r="K39" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L39" s="3" t="s">
+      <c r="M39" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M39" s="3"/>
       <c r="N39" s="3"/>
-      <c r="O39" s="3">
+      <c r="P39" s="3">
         <v>7</v>
       </c>
-      <c r="P39" s="1" t="s">
+      <c r="Q39" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Q39" s="1" t="s">
+      <c r="R39" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="R39" s="1">
+      <c r="S39" s="1">
         <v>35</v>
       </c>
-      <c r="S39" s="7" t="s">
+      <c r="T39" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="T39" s="3" t="s">
+      <c r="U39" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>144</v>
       </c>
@@ -4742,6 +3803,9 @@
       </c>
       <c r="E40" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="G40" s="9"/>
       <c r="H40" s="1"/>
@@ -4754,31 +3818,30 @@
       <c r="K40" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L40" s="3" t="s">
+      <c r="M40" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M40" s="3"/>
       <c r="N40" s="3"/>
-      <c r="O40" s="3">
+      <c r="P40" s="3">
         <v>4</v>
       </c>
-      <c r="P40" s="1" t="s">
+      <c r="Q40" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q40" s="1" t="s">
+      <c r="R40" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R40" s="1">
+      <c r="S40" s="1">
         <v>36</v>
       </c>
-      <c r="S40" s="7" t="s">
+      <c r="T40" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="T40" s="3" t="s">
+      <c r="U40" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>145</v>
       </c>
@@ -4790,6 +3853,9 @@
       </c>
       <c r="E41" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="G41" s="9"/>
       <c r="H41" s="1"/>
@@ -4797,20 +3863,20 @@
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
-      <c r="M41" s="3"/>
+      <c r="M41" s="5"/>
       <c r="N41" s="3"/>
-      <c r="O41" s="6">
+      <c r="P41" s="6">
         <v>5</v>
       </c>
-      <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
-      <c r="R41" s="5">
+      <c r="R41" s="6"/>
+      <c r="S41" s="5">
         <v>37</v>
       </c>
-      <c r="S41" s="6"/>
       <c r="T41" s="6"/>
-    </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U41" s="6"/>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>146</v>
       </c>
@@ -4822,6 +3888,9 @@
       </c>
       <c r="E42" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -4829,18 +3898,18 @@
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
-      <c r="M42" s="3"/>
+      <c r="M42" s="5"/>
       <c r="N42" s="3"/>
-      <c r="O42" s="6"/>
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
-      <c r="R42" s="5">
+      <c r="R42" s="6"/>
+      <c r="S42" s="5">
         <v>38</v>
       </c>
-      <c r="S42" s="6"/>
       <c r="T42" s="6"/>
-    </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U42" s="6"/>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>147</v>
       </c>
@@ -4852,6 +3921,9 @@
       </c>
       <c r="E43" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
@@ -4863,28 +3935,28 @@
       <c r="K43" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L43" s="3" t="s">
+      <c r="M43" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M43" s="3"/>
       <c r="N43" s="3"/>
-      <c r="P43" s="1" t="s">
+      <c r="P43" s="3"/>
+      <c r="Q43" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q43" s="1" t="s">
+      <c r="R43" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R43" s="1">
+      <c r="S43" s="1">
         <v>39</v>
       </c>
-      <c r="S43" s="7" t="s">
+      <c r="T43" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="T43" s="3" t="s">
+      <c r="U43" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>148</v>
       </c>
@@ -4896,12 +3968,15 @@
       </c>
       <c r="E44" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="J44" s="3"/>
       <c r="O44" s="1"/>
       <c r="P44" s="3"/>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>149</v>
       </c>
@@ -4918,7 +3993,7 @@
       <c r="O45" s="1"/>
       <c r="P45" s="3"/>
     </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>150</v>
       </c>
@@ -4935,7 +4010,7 @@
       <c r="O46" s="1"/>
       <c r="P46" s="3"/>
     </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>151</v>
       </c>
@@ -4953,7 +4028,7 @@
       <c r="O47" s="1"/>
       <c r="P47" s="3"/>
     </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>152</v>
       </c>
@@ -5061,577 +4136,170 @@
       <c r="P53" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O4:T35">
-    <sortCondition ref="Q4:Q35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P4:U35">
+    <sortCondition ref="R4:R35"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="K7:K8">
-    <cfRule type="expression" dxfId="175" priority="217">
-      <formula>K7="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7 S27 S29:S30 S36:S37 E8:E18 E25 E37:E46 F4:F24 F37:F53">
-    <cfRule type="expression" dxfId="174" priority="216" stopIfTrue="1">
+  <conditionalFormatting sqref="E4:E7 F13:F24 F37:F40 L4:L7">
+    <cfRule type="expression" dxfId="37" priority="68" stopIfTrue="1">
       <formula>E4="Avoid"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 S27 S29:S30 S36:S37 E8:E18 E25 E37:E46 F4:F24 F37:F53">
-    <cfRule type="expression" dxfId="173" priority="213">
-      <formula>E4="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="172" priority="215">
+  <conditionalFormatting sqref="E4:E18 L4:L8">
+    <cfRule type="expression" dxfId="36" priority="69">
       <formula>E4="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
-    <cfRule type="expression" dxfId="171" priority="214" stopIfTrue="1">
+  <conditionalFormatting sqref="E4:E25 L4:L6">
+    <cfRule type="expression" dxfId="35" priority="55">
+      <formula>E4="When Necessary"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19:E24">
+    <cfRule type="expression" dxfId="34" priority="56" stopIfTrue="1">
+      <formula>E19="Avoid"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19:E25">
+    <cfRule type="expression" dxfId="33" priority="57">
+      <formula>E19="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37:E53 F13:F24 F37:F40">
+    <cfRule type="expression" dxfId="32" priority="46">
+      <formula>E13="When Necessary"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="48">
+      <formula>E13="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47:E53">
+    <cfRule type="expression" dxfId="30" priority="47" stopIfTrue="1">
+      <formula>E47="Avoid"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F37:F40 T27 T29:T30 T36:T37 E8:E18 E25 E37:E46 F44:F53">
+    <cfRule type="expression" dxfId="29" priority="219" stopIfTrue="1">
+      <formula>E8="Avoid"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F37:F40 F44:F53">
+    <cfRule type="expression" dxfId="28" priority="216">
+      <formula>F37="When Necessary"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="218">
+      <formula>F37="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:K6">
+    <cfRule type="expression" dxfId="26" priority="195">
+      <formula>K4="When Necessary"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:K7">
+    <cfRule type="expression" dxfId="25" priority="196" stopIfTrue="1">
       <formula>K4="Avoid"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="170" priority="210">
-      <formula>K6="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="169" priority="212">
-      <formula>K6="OK"</formula>
+  <conditionalFormatting sqref="K4:K8">
+    <cfRule type="expression" dxfId="24" priority="197">
+      <formula>K4="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="168" priority="211" stopIfTrue="1">
-      <formula>K6="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="167" priority="207">
+  <conditionalFormatting sqref="K9:L22 K43:L43 K24:L40 K23">
+    <cfRule type="expression" dxfId="23" priority="192">
       <formula>K9="When Necessary"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="209">
+    <cfRule type="expression" dxfId="22" priority="193" stopIfTrue="1">
+      <formula>K9="Avoid"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="194">
       <formula>K9="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="165" priority="208" stopIfTrue="1">
-      <formula>K9="Avoid"</formula>
+  <conditionalFormatting sqref="T4:T15">
+    <cfRule type="expression" dxfId="20" priority="108">
+      <formula>T4="When Necessary"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="109" stopIfTrue="1">
+      <formula>T4="Avoid"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="110">
+      <formula>T4="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="164" priority="192">
-      <formula>K5="When Necessary"</formula>
+  <conditionalFormatting sqref="T17:T23">
+    <cfRule type="expression" dxfId="17" priority="141">
+      <formula>T17="When Necessary"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="194">
-      <formula>K5="OK"</formula>
+    <cfRule type="expression" dxfId="16" priority="142" stopIfTrue="1">
+      <formula>T17="Avoid"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="143">
+      <formula>T17="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="162" priority="193" stopIfTrue="1">
-      <formula>K5="Avoid"</formula>
+  <conditionalFormatting sqref="T25:T26">
+    <cfRule type="expression" dxfId="14" priority="169" stopIfTrue="1">
+      <formula>T25="Avoid"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K10:K40 K43">
-    <cfRule type="expression" dxfId="161" priority="189">
-      <formula>K10="When Necessary"</formula>
+  <conditionalFormatting sqref="T25:T27">
+    <cfRule type="expression" dxfId="13" priority="168">
+      <formula>T25="When Necessary"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="191">
-      <formula>K10="OK"</formula>
+    <cfRule type="expression" dxfId="12" priority="170">
+      <formula>T25="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K10:K40 K43">
-    <cfRule type="expression" dxfId="159" priority="190" stopIfTrue="1">
-      <formula>K10="Avoid"</formula>
+  <conditionalFormatting sqref="T29:T31">
+    <cfRule type="expression" dxfId="11" priority="165">
+      <formula>T29="When Necessary"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="167">
+      <formula>T29="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4">
-    <cfRule type="expression" dxfId="158" priority="186">
-      <formula>S4="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="157" priority="188">
-      <formula>S4="OK"</formula>
+  <conditionalFormatting sqref="T31">
+    <cfRule type="expression" dxfId="9" priority="166" stopIfTrue="1">
+      <formula>T31="Avoid"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4">
-    <cfRule type="expression" dxfId="156" priority="187" stopIfTrue="1">
-      <formula>S4="Avoid"</formula>
+  <conditionalFormatting sqref="T36:T40">
+    <cfRule type="expression" dxfId="8" priority="114">
+      <formula>T36="When Necessary"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="116">
+      <formula>T36="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S5">
-    <cfRule type="expression" dxfId="155" priority="183">
-      <formula>S5="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="154" priority="185">
-      <formula>S5="OK"</formula>
+  <conditionalFormatting sqref="T38:T40">
+    <cfRule type="expression" dxfId="6" priority="115" stopIfTrue="1">
+      <formula>T38="Avoid"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S5">
-    <cfRule type="expression" dxfId="153" priority="184" stopIfTrue="1">
-      <formula>S5="Avoid"</formula>
+  <conditionalFormatting sqref="T43">
+    <cfRule type="expression" dxfId="5" priority="111">
+      <formula>T43="When Necessary"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="112" stopIfTrue="1">
+      <formula>T43="Avoid"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="113">
+      <formula>T43="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8">
-    <cfRule type="expression" dxfId="152" priority="180">
-      <formula>S8="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="151" priority="182">
-      <formula>S8="OK"</formula>
+  <conditionalFormatting sqref="L23">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>L23="Avoid"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8">
-    <cfRule type="expression" dxfId="150" priority="181" stopIfTrue="1">
-      <formula>S8="Avoid"</formula>
+  <conditionalFormatting sqref="L23">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>L23="When Necessary"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S6">
-    <cfRule type="expression" dxfId="149" priority="177">
-      <formula>S6="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="148" priority="179">
-      <formula>S6="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S6">
-    <cfRule type="expression" dxfId="147" priority="178" stopIfTrue="1">
-      <formula>S6="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S15">
-    <cfRule type="expression" dxfId="146" priority="174">
-      <formula>S15="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="145" priority="176">
-      <formula>S15="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S15">
-    <cfRule type="expression" dxfId="144" priority="175" stopIfTrue="1">
-      <formula>S15="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S23">
-    <cfRule type="expression" dxfId="143" priority="171">
-      <formula>S23="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="142" priority="173">
-      <formula>S23="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S23">
-    <cfRule type="expression" dxfId="141" priority="172" stopIfTrue="1">
-      <formula>S23="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S26">
-    <cfRule type="expression" dxfId="140" priority="168">
-      <formula>S26="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="139" priority="170">
-      <formula>S26="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S26">
-    <cfRule type="expression" dxfId="138" priority="169" stopIfTrue="1">
-      <formula>S26="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S25">
-    <cfRule type="expression" dxfId="137" priority="165">
-      <formula>S25="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="136" priority="167">
-      <formula>S25="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S25">
-    <cfRule type="expression" dxfId="135" priority="166" stopIfTrue="1">
-      <formula>S25="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S31">
-    <cfRule type="expression" dxfId="134" priority="162">
-      <formula>S31="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="133" priority="164">
-      <formula>S31="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S31">
-    <cfRule type="expression" dxfId="132" priority="163" stopIfTrue="1">
-      <formula>S31="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S38">
-    <cfRule type="expression" dxfId="131" priority="159">
-      <formula>S38="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="130" priority="161">
-      <formula>S38="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S38">
-    <cfRule type="expression" dxfId="129" priority="160" stopIfTrue="1">
-      <formula>S38="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S39">
-    <cfRule type="expression" dxfId="128" priority="156">
-      <formula>S39="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="127" priority="158">
-      <formula>S39="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S39">
-    <cfRule type="expression" dxfId="126" priority="157" stopIfTrue="1">
-      <formula>S39="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S17">
-    <cfRule type="expression" dxfId="125" priority="153">
-      <formula>S17="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="124" priority="155">
-      <formula>S17="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S17">
-    <cfRule type="expression" dxfId="123" priority="154" stopIfTrue="1">
-      <formula>S17="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S22">
-    <cfRule type="expression" dxfId="122" priority="150">
-      <formula>S22="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="121" priority="152">
-      <formula>S22="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S22">
-    <cfRule type="expression" dxfId="120" priority="151" stopIfTrue="1">
-      <formula>S22="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S18">
-    <cfRule type="expression" dxfId="119" priority="147">
-      <formula>S18="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="149">
-      <formula>S18="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S18">
-    <cfRule type="expression" dxfId="117" priority="148" stopIfTrue="1">
-      <formula>S18="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S19">
-    <cfRule type="expression" dxfId="116" priority="144">
-      <formula>S19="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="146">
-      <formula>S19="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S19">
-    <cfRule type="expression" dxfId="114" priority="145" stopIfTrue="1">
-      <formula>S19="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S20">
-    <cfRule type="expression" dxfId="113" priority="141">
-      <formula>S20="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="112" priority="143">
-      <formula>S20="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S20">
-    <cfRule type="expression" dxfId="111" priority="142" stopIfTrue="1">
-      <formula>S20="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S21">
-    <cfRule type="expression" dxfId="110" priority="138">
-      <formula>S21="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="140">
-      <formula>S21="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S21">
-    <cfRule type="expression" dxfId="108" priority="139" stopIfTrue="1">
-      <formula>S21="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S9">
-    <cfRule type="expression" dxfId="107" priority="135">
-      <formula>S9="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="137">
-      <formula>S9="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S9">
-    <cfRule type="expression" dxfId="105" priority="136" stopIfTrue="1">
-      <formula>S9="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S14">
-    <cfRule type="expression" dxfId="104" priority="132">
-      <formula>S14="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="134">
-      <formula>S14="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S14">
-    <cfRule type="expression" dxfId="102" priority="133" stopIfTrue="1">
-      <formula>S14="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S10">
-    <cfRule type="expression" dxfId="101" priority="129">
-      <formula>S10="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="131">
-      <formula>S10="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S10">
-    <cfRule type="expression" dxfId="99" priority="130" stopIfTrue="1">
-      <formula>S10="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
-    <cfRule type="expression" dxfId="98" priority="126">
-      <formula>S11="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="97" priority="128">
-      <formula>S11="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
-    <cfRule type="expression" dxfId="96" priority="127" stopIfTrue="1">
-      <formula>S11="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S12">
-    <cfRule type="expression" dxfId="95" priority="123">
-      <formula>S12="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="125">
-      <formula>S12="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S12">
-    <cfRule type="expression" dxfId="93" priority="124" stopIfTrue="1">
-      <formula>S12="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S13">
-    <cfRule type="expression" dxfId="92" priority="120">
-      <formula>S13="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="122">
-      <formula>S13="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S13">
-    <cfRule type="expression" dxfId="90" priority="121" stopIfTrue="1">
-      <formula>S13="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S40">
-    <cfRule type="expression" dxfId="89" priority="111">
-      <formula>S40="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="113">
-      <formula>S40="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S40">
-    <cfRule type="expression" dxfId="87" priority="112" stopIfTrue="1">
-      <formula>S40="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S43">
-    <cfRule type="expression" dxfId="86" priority="108">
-      <formula>S43="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="110">
-      <formula>S43="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S43">
-    <cfRule type="expression" dxfId="84" priority="109" stopIfTrue="1">
-      <formula>S43="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S7">
-    <cfRule type="expression" dxfId="83" priority="105">
-      <formula>S7="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="107">
-      <formula>S7="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S7">
-    <cfRule type="expression" dxfId="81" priority="106" stopIfTrue="1">
-      <formula>S7="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23:E24 E47">
-    <cfRule type="expression" dxfId="80" priority="88">
-      <formula>E23="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="79" priority="90">
-      <formula>E23="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23:E24 E47">
-    <cfRule type="expression" dxfId="78" priority="89" stopIfTrue="1">
-      <formula>E23="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
-    <cfRule type="expression" dxfId="77" priority="85">
-      <formula>E48="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="87">
-      <formula>E48="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
-    <cfRule type="expression" dxfId="75" priority="86" stopIfTrue="1">
-      <formula>E48="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="74" priority="73">
-      <formula>E4="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="75">
-      <formula>E4="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="72" priority="74" stopIfTrue="1">
-      <formula>E4="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="71" priority="70">
-      <formula>E5="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="72">
-      <formula>E5="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="69" priority="71" stopIfTrue="1">
-      <formula>E5="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="68" priority="67">
-      <formula>E6="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="69">
-      <formula>E6="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="66" priority="68" stopIfTrue="1">
-      <formula>E6="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="65" priority="64">
-      <formula>E7="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="66">
-      <formula>E7="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="63" priority="65" stopIfTrue="1">
-      <formula>E7="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="62" priority="61">
-      <formula>E19="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="63">
-      <formula>E19="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="60" priority="62" stopIfTrue="1">
-      <formula>E19="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="59" priority="58">
-      <formula>E20="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="60">
-      <formula>E20="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="57" priority="59" stopIfTrue="1">
-      <formula>E20="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="expression" dxfId="56" priority="55">
-      <formula>E21="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="55" priority="57">
-      <formula>E21="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="expression" dxfId="54" priority="56" stopIfTrue="1">
-      <formula>E21="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="53" priority="52">
-      <formula>E22="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="54">
-      <formula>E22="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="51" priority="53" stopIfTrue="1">
-      <formula>E22="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49:E52">
-    <cfRule type="expression" dxfId="50" priority="46">
-      <formula>E49="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="48">
-      <formula>E49="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49:E52">
-    <cfRule type="expression" dxfId="48" priority="47" stopIfTrue="1">
-      <formula>E49="Avoid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="expression" dxfId="47" priority="43">
-      <formula>E53="When Necessary"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="45">
-      <formula>E53="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="expression" dxfId="45" priority="44" stopIfTrue="1">
-      <formula>E53="Avoid"</formula>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>L23="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>